<commit_message>
fixed 2 problems: missed a few spots to multiple eggs by female prop and re-ran with corrected inital condition
</commit_message>
<xml_diff>
--- a/data/RAW/Catch-Effort_Data_Tables_from_reports .xlsx
+++ b/data/RAW/Catch-Effort_Data_Tables_from_reports .xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="160" yWindow="1180" windowWidth="28640" windowHeight="15540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="160" yWindow="1180" windowWidth="28640" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="7_spp_GN_enmalle" sheetId="1" r:id="rId1"/>
@@ -1565,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1641,172 +1641,197 @@
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
+      <c r="B7" s="82"/>
       <c r="C7">
-        <v>166</v>
+        <f>C6*1000/ezfureza_por_arte_y_spp_2012!$K$9</f>
+        <v>238839.54019300893</v>
       </c>
       <c r="D7">
-        <v>258</v>
+        <f>D6*1000/ezfureza_por_arte_y_spp_2012!$K$9</f>
+        <v>223126.41254873204</v>
       </c>
       <c r="E7">
-        <v>232</v>
+        <f>E6*1000/ezfureza_por_arte_y_spp_2012!$K$9</f>
+        <v>161321.4438145762</v>
       </c>
       <c r="F7">
-        <v>142</v>
+        <f>F6*1000/ezfureza_por_arte_y_spp_2012!$K$9</f>
+        <v>231506.74729234638</v>
       </c>
       <c r="G7">
-        <v>199</v>
-      </c>
-      <c r="H7" s="2">
-        <v>9.0999999999999998E-2</v>
-      </c>
+        <f>G6*1000/ezfureza_por_arte_y_spp_2012!$K$9</f>
+        <v>213698.53596216589</v>
+      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>122</v>
+        <v>166</v>
       </c>
       <c r="D8">
-        <v>139</v>
+        <v>258</v>
       </c>
       <c r="E8">
-        <v>152</v>
+        <v>232</v>
       </c>
       <c r="F8">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="G8">
-        <v>141</v>
+        <v>199</v>
       </c>
       <c r="H8" s="2">
-        <v>6.4000000000000001E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="D9">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="E9">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="F9">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="G9">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="H9" s="2">
-        <v>6.2E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="D10">
-        <v>72</v>
+        <v>169</v>
       </c>
       <c r="E10">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F10">
-        <v>58</v>
+        <v>122</v>
       </c>
       <c r="G10">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="H10" s="2">
-        <v>4.1000000000000002E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="D11">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E11">
-        <v>78</v>
+        <v>123</v>
       </c>
       <c r="F11">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="G11">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="H11" s="2">
-        <v>3.4000000000000002E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>98</v>
+      </c>
+      <c r="D12">
+        <v>78</v>
+      </c>
+      <c r="E12">
+        <v>78</v>
+      </c>
+      <c r="F12">
+        <v>47</v>
+      </c>
+      <c r="G12">
+        <v>75</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>51</v>
       </c>
-      <c r="D12">
+      <c r="D13">
         <v>89</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>84</v>
       </c>
-      <c r="F12">
+      <c r="F13">
         <v>69</v>
       </c>
-      <c r="G12">
+      <c r="G13">
         <v>73</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H13" s="2">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C14" s="5">
         <v>1783</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D14" s="5">
         <v>2178</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E14" s="5">
         <v>2485</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F14" s="5">
         <v>2349</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G14" s="5">
         <v>2199</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H14" s="6">
         <v>1</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5200,7 +5225,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>